<commit_message>
still shitty data yay
</commit_message>
<xml_diff>
--- a/data_error_analysis.xlsx
+++ b/data_error_analysis.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Different Planes" sheetId="2" r:id="rId1"/>
     <sheet name="Pileup Profiles" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Pileup Profiles 2" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Load</t>
   </si>
@@ -202,8 +202,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -315,7 +317,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -359,6 +361,7 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -402,6 +405,7 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1690,7 +1694,7 @@
   <dimension ref="C3:P34"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C1" sqref="C1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1767,7 +1771,7 @@
         <v>-2.2573363431151261</v>
       </c>
       <c r="J4" s="19">
-        <f>(H4-F4)/AVERAGE(H4,F4)*100</f>
+        <f t="shared" ref="J4:J18" si="0">(H4-F4)/AVERAGE(H4,F4)*100</f>
         <v>2.8571428571428399</v>
       </c>
       <c r="L4">
@@ -1810,11 +1814,11 @@
         <v>3.9E-2</v>
       </c>
       <c r="I5" s="19">
-        <f t="shared" ref="I5:I21" si="0">(G5-E5)/AVERAGE(E5,G5)*100</f>
+        <f t="shared" ref="I5:I21" si="1">(G5-E5)/AVERAGE(E5,G5)*100</f>
         <v>-3.9436619718309895</v>
       </c>
       <c r="J5" s="19">
-        <f>(H5-F5)/AVERAGE(H5,F5)*100</f>
+        <f t="shared" si="0"/>
         <v>-52.830188679245282</v>
       </c>
       <c r="L5">
@@ -1857,11 +1861,11 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="I6" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.218649517684899</v>
       </c>
       <c r="J6" s="19">
-        <f>(H6-F6)/AVERAGE(H6,F6)*100</f>
+        <f t="shared" si="0"/>
         <v>60.740740740740726</v>
       </c>
       <c r="L6">
@@ -1904,11 +1908,11 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="I7" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-12.541254125412552</v>
       </c>
       <c r="J7" s="19">
-        <f>(H7-F7)/AVERAGE(H7,F7)*100</f>
+        <f t="shared" si="0"/>
         <v>-11.76470588235293</v>
       </c>
       <c r="L7">
@@ -1951,11 +1955,11 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="I8" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J8" s="19">
-        <f>(H8-F8)/AVERAGE(H8,F8)*100</f>
+        <f t="shared" si="0"/>
         <v>38.202247191011239</v>
       </c>
       <c r="L8">
@@ -1998,11 +2002,11 @@
         <v>0.127</v>
       </c>
       <c r="I9" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2371364653243866</v>
       </c>
       <c r="J9" s="19">
-        <f>(H9-F9)/AVERAGE(H9,F9)*100</f>
+        <f t="shared" si="0"/>
         <v>-48.80952380952381</v>
       </c>
       <c r="M9" s="6"/>
@@ -2028,11 +2032,11 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="I10" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8109965635738874</v>
       </c>
       <c r="J10" s="19">
-        <f>(H10-F10)/AVERAGE(H10,F10)*100</f>
+        <f t="shared" si="0"/>
         <v>-16.393442622950825</v>
       </c>
     </row>
@@ -2056,11 +2060,11 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="I11" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-37.908496732026144</v>
       </c>
       <c r="J11" s="19">
-        <f>(H11-F11)/AVERAGE(H11,F11)*100</f>
+        <f t="shared" si="0"/>
         <v>1.1363636363636374</v>
       </c>
     </row>
@@ -2084,11 +2088,11 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="I12" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-17.294900221729495</v>
       </c>
       <c r="J12" s="19">
-        <f>(H12-F12)/AVERAGE(H12,F12)*100</f>
+        <f t="shared" si="0"/>
         <v>-54.411764705882334</v>
       </c>
     </row>
@@ -2112,11 +2116,11 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="I13" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.6984352773826492</v>
       </c>
       <c r="J13" s="19">
-        <f>(H13-F13)/AVERAGE(H13,F13)*100</f>
+        <f t="shared" si="0"/>
         <v>-46.616541353383468</v>
       </c>
     </row>
@@ -2140,11 +2144,11 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="I14" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.8495575221238862</v>
       </c>
       <c r="J14" s="19">
-        <f>(H14-F14)/AVERAGE(H14,F14)*100</f>
+        <f t="shared" si="0"/>
         <v>-16.822429906542055</v>
       </c>
     </row>
@@ -2168,11 +2172,11 @@
         <v>0.04</v>
       </c>
       <c r="I15" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.8985507246376838</v>
       </c>
       <c r="J15" s="19">
-        <f>(H15-F15)/AVERAGE(H15,F15)*100</f>
+        <f t="shared" si="0"/>
         <v>-31.578947368421051</v>
       </c>
     </row>
@@ -2196,11 +2200,11 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="I16" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0874785591766751</v>
       </c>
       <c r="J16" s="19">
-        <f>(H16-F16)/AVERAGE(H16,F16)*100</f>
+        <f t="shared" si="0"/>
         <v>34.482758620689658</v>
       </c>
     </row>
@@ -2224,11 +2228,11 @@
         <v>0.498</v>
       </c>
       <c r="I17" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.1286307053941993</v>
       </c>
       <c r="J17" s="19">
-        <f>(H17-F17)/AVERAGE(H17,F17)*100</f>
+        <f t="shared" si="0"/>
         <v>3.0581039755351709</v>
       </c>
     </row>
@@ -2252,11 +2256,11 @@
         <v>0.11</v>
       </c>
       <c r="I18" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.4054054054054106</v>
       </c>
       <c r="J18" s="19">
-        <f>(H18-F18)/AVERAGE(H18,F18)*100</f>
+        <f t="shared" si="0"/>
         <v>-3.5714285714285747</v>
       </c>
     </row>
@@ -2294,7 +2298,7 @@
         <v>0.123</v>
       </c>
       <c r="I20" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81632653061224569</v>
       </c>
       <c r="J20" s="19">
@@ -2322,7 +2326,7 @@
         <v>0.19900000000000001</v>
       </c>
       <c r="I21" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-85.009487666034161</v>
       </c>
       <c r="J21" s="19">
@@ -2378,11 +2382,11 @@
         <v>0.151</v>
       </c>
       <c r="I23" s="19">
-        <f t="shared" ref="I23:I27" si="1">(H23-E23)/AVERAGE(H23,E23)*100</f>
+        <f t="shared" ref="I23:I27" si="2">(H23-E23)/AVERAGE(H23,E23)*100</f>
         <v>8.9965397923875319</v>
       </c>
       <c r="J23" s="19">
-        <f t="shared" ref="J23:J27" si="2">(G23-F23)/AVERAGE(G23,F23)*100</f>
+        <f t="shared" ref="J23:J27" si="3">(G23-F23)/AVERAGE(G23,F23)*100</f>
         <v>1.0526315789473693</v>
       </c>
     </row>
@@ -2406,11 +2410,11 @@
         <v>0.126</v>
       </c>
       <c r="I24" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24.390243902439025</v>
       </c>
       <c r="J24" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-11.387900355871876</v>
       </c>
     </row>
@@ -2434,11 +2438,11 @@
         <v>0.21</v>
       </c>
       <c r="I25" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-48.375451263537904</v>
       </c>
       <c r="J25" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.778025241276911</v>
       </c>
     </row>
@@ -2462,11 +2466,11 @@
         <v>0.14099999999999999</v>
       </c>
       <c r="I26" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-9.4594594594594685</v>
       </c>
       <c r="J26" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-45.916795069337446</v>
       </c>
     </row>
@@ -2490,11 +2494,11 @@
         <v>0.215</v>
       </c>
       <c r="I27" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108.24372759856628</v>
       </c>
       <c r="J27" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49.558941459502819</v>
       </c>
     </row>
@@ -2522,7 +2526,7 @@
         <v>-51.263537906137181</v>
       </c>
       <c r="J28" s="19">
-        <f>(H28-F28)/AVERAGE(H28,F28)*100</f>
+        <f t="shared" ref="J28:J33" si="4">(H28-F28)/AVERAGE(H28,F28)*100</f>
         <v>17.791411042944784</v>
       </c>
     </row>
@@ -2546,11 +2550,11 @@
         <v>0.26300000000000001</v>
       </c>
       <c r="I29" s="19">
-        <f t="shared" ref="I29:I33" si="3">(G29-E29)/AVERAGE(E29,G29)*100</f>
+        <f t="shared" ref="I29:I33" si="5">(G29-E29)/AVERAGE(E29,G29)*100</f>
         <v>37.054631828978614</v>
       </c>
       <c r="J29" s="19">
-        <f>(H29-F29)/AVERAGE(H29,F29)*100</f>
+        <f t="shared" si="4"/>
         <v>18.711018711018717</v>
       </c>
     </row>
@@ -2574,11 +2578,11 @@
         <v>0.314</v>
       </c>
       <c r="I30" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.000000000000002</v>
       </c>
       <c r="J30" s="19">
-        <f>(H30-F30)/AVERAGE(H30,F30)*100</f>
+        <f t="shared" si="4"/>
         <v>48.221343873517789</v>
       </c>
     </row>
@@ -2602,11 +2606,11 @@
         <v>0.38600000000000001</v>
       </c>
       <c r="I31" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-12.389380530973444</v>
       </c>
       <c r="J31" s="19">
-        <f>(H31-F31)/AVERAGE(H31,F31)*100</f>
+        <f t="shared" si="4"/>
         <v>102.15264187866929</v>
       </c>
     </row>
@@ -2630,11 +2634,11 @@
         <v>0.52900000000000003</v>
       </c>
       <c r="I32" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-13.333333333333334</v>
       </c>
       <c r="J32" s="19">
-        <f>(H32-F32)/AVERAGE(H32,F32)*100</f>
+        <f t="shared" si="4"/>
         <v>113.48148148148147</v>
       </c>
     </row>
@@ -2658,11 +2662,11 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="I33" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-77.858176555716369</v>
       </c>
       <c r="J33" s="19">
-        <f>(H33-F33)/AVERAGE(H33,F33)*100</f>
+        <f t="shared" si="4"/>
         <v>-41.452344931921331</v>
       </c>
     </row>
@@ -2689,12 +2693,1460 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C3:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:16">
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="3:16">
+      <c r="C4" s="7">
+        <v>490</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.122</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="I4" s="19">
+        <f>(G4-E4)/AVERAGE(E4,G4)*100</f>
+        <v>7.1146245059288598</v>
+      </c>
+      <c r="J4" s="19">
+        <f t="shared" ref="J4:J53" si="0">(H4-F4)/AVERAGE(H4,F4)*100</f>
+        <v>20.532319391634974</v>
+      </c>
+      <c r="L4">
+        <v>490</v>
+      </c>
+      <c r="M4" s="3">
+        <f>AVERAGE(E4:F9)*1000</f>
+        <v>115.08333333333333</v>
+      </c>
+      <c r="N4" s="3">
+        <f>STDEV(E4:F9)*1000</f>
+        <v>40.27960985035687</v>
+      </c>
+      <c r="O4" s="3">
+        <f>AVERAGE(G4:H9)*1000</f>
+        <v>90.666666666666657</v>
+      </c>
+      <c r="P4" s="3">
+        <f>STDEV(G4:H9)*1000</f>
+        <v>42.110964526276739</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16">
+      <c r="C5" s="7">
+        <v>490</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="H5" s="7">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I5" s="19">
+        <f t="shared" ref="I5:I53" si="1">(G5-E5)/AVERAGE(E5,G5)*100</f>
+        <v>-4.8780487804878092</v>
+      </c>
+      <c r="J5" s="19">
+        <f t="shared" si="0"/>
+        <v>-74.747474747474755</v>
+      </c>
+      <c r="L5">
+        <v>981</v>
+      </c>
+      <c r="M5" s="3">
+        <f>AVERAGE(E14:F19)*1000</f>
+        <v>141.16666666666669</v>
+      </c>
+      <c r="N5" s="3">
+        <f>STDEV(E14:F19)*1000</f>
+        <v>55.43027287967422</v>
+      </c>
+      <c r="O5" s="3">
+        <f>AVERAGE(G14:H19)*1000</f>
+        <v>79</v>
+      </c>
+      <c r="P5" s="3">
+        <f>STDEV(G14:H19)*1000</f>
+        <v>45.569128305745032</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16">
+      <c r="C6" s="7">
+        <v>490</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="I6" s="19">
+        <f t="shared" si="1"/>
+        <v>-66.666666666666671</v>
+      </c>
+      <c r="J6" s="19">
+        <f t="shared" si="0"/>
+        <v>-37.751004016064243</v>
+      </c>
+      <c r="L6">
+        <v>1961</v>
+      </c>
+      <c r="M6" s="3">
+        <f>AVERAGE(E24:F29)*1000</f>
+        <v>268.75</v>
+      </c>
+      <c r="N6" s="3">
+        <f>STDEV(E24:F29)*1000</f>
+        <v>160.31736989767859</v>
+      </c>
+      <c r="O6" s="3" t="e">
+        <f>AVERAGE(G24:H29)*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P6" s="3" t="e">
+        <f>STDEV(G24:H29)*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16">
+      <c r="C7" s="7">
+        <v>490</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="F7" s="8">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="H7" s="7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I7" s="19">
+        <f t="shared" si="1"/>
+        <v>12.31671554252199</v>
+      </c>
+      <c r="J7" s="19">
+        <f t="shared" si="0"/>
+        <v>-26.589595375722553</v>
+      </c>
+      <c r="L7">
+        <v>2942</v>
+      </c>
+      <c r="M7" s="3">
+        <f>AVERAGE(E34:F39)*1000</f>
+        <v>375.33333333333331</v>
+      </c>
+      <c r="N7" s="3">
+        <f>STDEV(E34:F39)*1000</f>
+        <v>163.73500393975493</v>
+      </c>
+      <c r="O7" s="3" t="e">
+        <f>AVERAGE(G34:H39)*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P7" s="3" t="e">
+        <f>STDEV(G34:H39)*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16">
+      <c r="C8" s="7">
+        <v>490</v>
+      </c>
+      <c r="D8" s="7">
+        <v>5</v>
+      </c>
+      <c r="E8" s="8">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.157</v>
+      </c>
+      <c r="G8" s="7">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="I8" s="19">
+        <f t="shared" si="1"/>
+        <v>14.705882352941169</v>
+      </c>
+      <c r="J8" s="19">
+        <f t="shared" si="0"/>
+        <v>-48.221343873517789</v>
+      </c>
+      <c r="L8">
+        <v>4903</v>
+      </c>
+      <c r="M8" s="3">
+        <f>AVERAGE(E44:F49)*1000</f>
+        <v>375.58333333333331</v>
+      </c>
+      <c r="N8" s="3">
+        <f>STDEV(E44:F49)*1000</f>
+        <v>81.304655276909074</v>
+      </c>
+      <c r="O8" s="3" t="e">
+        <f>AVERAGE(G44:H49)*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P8" s="3" t="e">
+        <f>STDEV(G44:H49)*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16">
+      <c r="C9" s="7">
+        <v>490</v>
+      </c>
+      <c r="D9" s="7">
+        <v>6</v>
+      </c>
+      <c r="E9" s="8">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G9" s="7">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H9" s="7">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="I9" s="19">
+        <f t="shared" si="1"/>
+        <v>-5.9701492537313481</v>
+      </c>
+      <c r="J9" s="19">
+        <f t="shared" si="0"/>
+        <v>-94.827586206896569</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="3:16">
+      <c r="C10" s="7">
+        <v>490</v>
+      </c>
+      <c r="D10" s="7">
+        <v>7</v>
+      </c>
+      <c r="E10" s="8">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="G10" s="7">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="H10" s="7">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="I10" s="19">
+        <f t="shared" si="1"/>
+        <v>3.8709677419354875</v>
+      </c>
+      <c r="J10" s="19">
+        <f t="shared" si="0"/>
+        <v>-36.68639053254438</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="3:16">
+      <c r="C11" s="7">
+        <v>490</v>
+      </c>
+      <c r="D11" s="7">
+        <v>8</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F11" s="8">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G11" s="7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H11" s="7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="I11" s="19">
+        <f t="shared" si="1"/>
+        <v>-31.325301204819272</v>
+      </c>
+      <c r="J11" s="19">
+        <f t="shared" si="0"/>
+        <v>-5.8479532163742585</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="3:16">
+      <c r="C12" s="7">
+        <v>490</v>
+      </c>
+      <c r="D12" s="7">
+        <v>9</v>
+      </c>
+      <c r="E12" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F12" s="8">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G12" s="7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H12" s="7">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="I12" s="19">
+        <f t="shared" si="1"/>
+        <v>-158.97435897435898</v>
+      </c>
+      <c r="J12" s="19">
+        <f t="shared" si="0"/>
+        <v>13.49693251533742</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="3:16">
+      <c r="C13" s="7">
+        <v>490</v>
+      </c>
+      <c r="D13" s="7">
+        <v>10</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.122</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G13" s="7">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H13" s="7">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="I13" s="19">
+        <f t="shared" si="1"/>
+        <v>-114.83870967741936</v>
+      </c>
+      <c r="J13" s="19">
+        <f t="shared" si="0"/>
+        <v>-122.64150943396226</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="3:16">
+      <c r="C14" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0.215</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="H14" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I14" s="19">
+        <f t="shared" si="1"/>
+        <v>1.7595307917888419</v>
+      </c>
+      <c r="J14" s="19">
+        <f t="shared" si="0"/>
+        <v>-126.99619771863115</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16">
+      <c r="C15" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2</v>
+      </c>
+      <c r="E15" s="10">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0.18</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0.105</v>
+      </c>
+      <c r="I15" s="19">
+        <f t="shared" si="1"/>
+        <v>112.5</v>
+      </c>
+      <c r="J15" s="19">
+        <f t="shared" si="0"/>
+        <v>-52.631578947368418</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16">
+      <c r="C16" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D16" s="9">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="F16" s="10">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G16" s="9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H16" s="9">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="I16" s="19">
+        <f t="shared" si="1"/>
+        <v>-134.02061855670101</v>
+      </c>
+      <c r="J16" s="19">
+        <f t="shared" si="0"/>
+        <v>36.111111111111121</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10">
+      <c r="C17" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D17" s="9">
+        <v>4</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G17" s="9">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I17" s="19">
+        <f t="shared" si="1"/>
+        <v>-141.10429447852761</v>
+      </c>
+      <c r="J17" s="19">
+        <f t="shared" si="0"/>
+        <v>6.4981949458483612</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10">
+      <c r="C18" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D18" s="9">
+        <v>5</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="G18" s="9">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="H18" s="9">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I18" s="19">
+        <f t="shared" si="1"/>
+        <v>-66.666666666666671</v>
+      </c>
+      <c r="J18" s="19">
+        <f t="shared" si="0"/>
+        <v>-133.89830508474577</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10">
+      <c r="C19" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D19" s="9">
+        <v>6</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="F19" s="10">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G19" s="9">
+        <v>4.7E-2</v>
+      </c>
+      <c r="H19" s="9">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="I19" s="19">
+        <f t="shared" si="1"/>
+        <v>-103.58974358974358</v>
+      </c>
+      <c r="J19" s="19">
+        <f t="shared" si="0"/>
+        <v>-31.707317073170728</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10">
+      <c r="C20" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D20" s="9">
+        <v>7</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G20" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="H20" s="9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="I20" s="19">
+        <f t="shared" si="1"/>
+        <v>-62.146892655367246</v>
+      </c>
+      <c r="J20" s="19">
+        <f t="shared" si="0"/>
+        <v>-74.226804123711347</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10">
+      <c r="C21" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D21" s="9">
+        <v>8</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.222</v>
+      </c>
+      <c r="F21" s="10">
+        <v>6.3E-2</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="H21" s="9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I21" s="19">
+        <f t="shared" si="1"/>
+        <v>-138.93129770992365</v>
+      </c>
+      <c r="J21" s="19">
+        <f t="shared" si="0"/>
+        <v>-9.9999999999999982</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10">
+      <c r="C22" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D22" s="9">
+        <v>9</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0.182</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="G22" s="9">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H22" s="9">
+        <v>6.3E-2</v>
+      </c>
+      <c r="I22" s="19">
+        <f t="shared" si="1"/>
+        <v>-92.369477911646584</v>
+      </c>
+      <c r="J22" s="19">
+        <f t="shared" si="0"/>
+        <v>-129.01408450704227</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10">
+      <c r="C23" s="9">
+        <v>980.7</v>
+      </c>
+      <c r="D23" s="9">
+        <v>10</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="F23" s="10">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0.191</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I23" s="19">
+        <f t="shared" si="1"/>
+        <v>7.6086956521739202</v>
+      </c>
+      <c r="J23" s="19">
+        <f t="shared" si="0"/>
+        <v>-89.908256880733944</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10">
+      <c r="C24" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D24" s="11">
+        <v>1</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J24" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10">
+      <c r="C25" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D25" s="11">
+        <v>2</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J25" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10">
+      <c r="C26" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D26" s="11">
+        <v>3</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0.114</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J26" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10">
+      <c r="C27" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D27" s="11">
+        <v>4</v>
+      </c>
+      <c r="E27" s="12">
+        <v>0.246</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J27" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10">
+      <c r="C28" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D28" s="11">
+        <v>5</v>
+      </c>
+      <c r="E28" s="12">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0.253</v>
+      </c>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J28" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10">
+      <c r="C29" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D29" s="11">
+        <v>6</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0.222</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0.63</v>
+      </c>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J29" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10">
+      <c r="C30" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D30" s="11">
+        <v>7</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0.223</v>
+      </c>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J30" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10">
+      <c r="C31" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D31" s="11">
+        <v>8</v>
+      </c>
+      <c r="E31" s="12">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F31" s="12">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J31" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10">
+      <c r="C32" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D32" s="11">
+        <v>9</v>
+      </c>
+      <c r="E32" s="12">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J32" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10">
+      <c r="C33" s="11">
+        <v>1961</v>
+      </c>
+      <c r="D33" s="11">
+        <v>10</v>
+      </c>
+      <c r="E33" s="12">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0.216</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J33" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10">
+      <c r="C34" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D34" s="14">
+        <v>1</v>
+      </c>
+      <c r="E34" s="15">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="F34" s="15">
+        <v>0.504</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J34" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10">
+      <c r="C35" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D35" s="14">
+        <v>2</v>
+      </c>
+      <c r="E35" s="15">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="F35" s="15">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J35" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10">
+      <c r="C36" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D36" s="14">
+        <v>3</v>
+      </c>
+      <c r="E36" s="15">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="F36" s="15">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J36" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10">
+      <c r="C37" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D37" s="14">
+        <v>4</v>
+      </c>
+      <c r="E37" s="15">
+        <v>0.316</v>
+      </c>
+      <c r="F37" s="15">
+        <v>0.77</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J37" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10">
+      <c r="C38" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D38" s="14">
+        <v>5</v>
+      </c>
+      <c r="E38" s="15">
+        <v>0.161</v>
+      </c>
+      <c r="F38" s="15">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J38" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10">
+      <c r="C39" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D39" s="14">
+        <v>6</v>
+      </c>
+      <c r="E39" s="15">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="F39" s="15">
+        <v>0.497</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J39" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10">
+      <c r="C40" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D40" s="14">
+        <v>7</v>
+      </c>
+      <c r="E40" s="15">
+        <v>0.156</v>
+      </c>
+      <c r="F40" s="15">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J40" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10">
+      <c r="C41" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D41" s="14">
+        <v>8</v>
+      </c>
+      <c r="E41" s="15">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="F41" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J41" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10">
+      <c r="C42" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D42" s="14">
+        <v>9</v>
+      </c>
+      <c r="E42" s="15">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="F42" s="15">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J42" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10">
+      <c r="C43" s="13">
+        <v>2942</v>
+      </c>
+      <c r="D43" s="14">
+        <v>10</v>
+      </c>
+      <c r="E43" s="15">
+        <v>0.373</v>
+      </c>
+      <c r="F43" s="15">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J43" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10">
+      <c r="C44" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D44" s="17">
+        <v>1</v>
+      </c>
+      <c r="E44" s="18">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="F44" s="18">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J44" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10">
+      <c r="C45" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D45" s="17">
+        <v>2</v>
+      </c>
+      <c r="E45" s="18">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="F45" s="18">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J45" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10">
+      <c r="C46" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D46" s="17">
+        <v>3</v>
+      </c>
+      <c r="E46" s="18">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="F46" s="18">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J46" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10">
+      <c r="C47" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D47" s="17">
+        <v>4</v>
+      </c>
+      <c r="E47" s="18">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="F47" s="18">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J47" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10">
+      <c r="C48" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D48" s="17">
+        <v>5</v>
+      </c>
+      <c r="E48" s="18">
+        <v>0.373</v>
+      </c>
+      <c r="F48" s="18">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J48" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10">
+      <c r="C49" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D49" s="17">
+        <v>6</v>
+      </c>
+      <c r="E49" s="18">
+        <v>0.312</v>
+      </c>
+      <c r="F49" s="18">
+        <v>0.499</v>
+      </c>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J49" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10">
+      <c r="C50" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D50" s="17">
+        <v>7</v>
+      </c>
+      <c r="E50" s="18">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="F50" s="18">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J50" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10">
+      <c r="C51" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D51" s="17">
+        <v>8</v>
+      </c>
+      <c r="E51" s="18">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="F51" s="18">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J51" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10">
+      <c r="C52" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D52" s="17">
+        <v>9</v>
+      </c>
+      <c r="E52" s="18">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="F52" s="18">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J52" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10">
+      <c r="C53" s="16">
+        <v>4903</v>
+      </c>
+      <c r="D53" s="17">
+        <v>10</v>
+      </c>
+      <c r="E53" s="18">
+        <v>0.621</v>
+      </c>
+      <c r="F53" s="18">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="19">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="J53" s="19">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10">
+      <c r="I54" s="20">
+        <f>AVERAGE(I4:J49)</f>
+        <v>-78.050681014269543</v>
+      </c>
+      <c r="J54" s="21">
+        <f>STDEV(I4:J49)</f>
+        <v>47.689760093131262</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>